<commit_message>
Bilder Lager und Öllauf
</commit_message>
<xml_diff>
--- a/Antriebslager-Berechnungen.xlsx
+++ b/Antriebslager-Berechnungen.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hopfm.tmb18\Documents\GitHub\KE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63713603-20DA-4FDF-8A62-6FF75BC8071F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37583B76-E891-4143-89F2-24D31615EFE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{1AF76359-922D-4612-B5D8-8695EF5B153C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="2" xr2:uid="{1AF76359-922D-4612-B5D8-8695EF5B153C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="QJ2" sheetId="1" r:id="rId1"/>
+    <sheet name="NU21" sheetId="2" r:id="rId2"/>
+    <sheet name="NU22" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -545,8 +546,268 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author xml:space="preserve">  </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{90F7202A-01BA-49A5-B909-1B76984D331E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Informationen zu diesem Programm:
+Berechnung der Lebensdauer und der statischen Kennzahl von Wälzlagern,
+außer Axial-Pendelrollenlager.
+Abschnitt:
+18.4
+Beispiele:
+18.1
+18.2, ohne Teil 1
+18.3
+Aufgaben:
+A18.1
+A18.2, nur Teil 2 und Teil 3, wobei die Drehzahl n = 229,2 min</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="superscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>-1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> getrennt 
+            berechnet werden muss.
+A18.3, wobei die  Drehzahl n = 302 min</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="superscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>-1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> getrennt berechnet werden muss.
+A18.4, ohne Teil 3
+A18.9
+A18.11, ohne Teil 3
+A18.13
+A18.17, ohne Grenzdrehzahl
+A18.21, ohne Grenzdrehzahl
+A18.23, wobei die Werte für X = 0,57 und Y = 0,93 nach Entsperren der Zelle
+              für den Wert X eingegeben werden müssen, ohne Grenzdrehzahl.
+A18.25, wobei bei der Berechnung der Schrägkugellager die Werte
+              für X = 0,35 und Y = 0,57 nach Entsperren der Zelle
+              für den Wert X eingegeben werden müssen.
+A18.30, nur Teil 1, wobei nach Entsperren der Zelle
+              für den Wert X = 0,67 eingegeben werden muss.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{C81079CA-939E-491B-BB8B-B83CA993CECC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>siehe ME, Abschnitt 18.5:
+für paarweise eingebaute Schrägkugellager in Tandem-, O- oder X-Anordnung ist der Tabellenwert von C mit 1,625 zu multiplizieren.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{7CAA2FD6-D313-4DA8-AD07-D989598C98C1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Die Belastungsgrößen F</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, F</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>a</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> und n sind konstant (stationärer Betrieb).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{C7623616-32AC-4C1C-9DBA-3389A691FF0E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">mittlerer Lagerdurchmesser = 0,5 (d + D)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B55" authorId="0" shapeId="0" xr:uid="{45203CD5-CD65-4D8B-9871-5F5B84EF078E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>siehe ME, Abschnitt 18.4:
+Allgemein strebt man für die Laufruhe und das Reibverhalten an:
+f</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 1,5 ... 2,5  bei hohen Ansprüchen
+f</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 1,0 ... 1,5  bei normalen Ansprüchen
+f</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 0,7 ... 1,0 bei geringen Ansprüchen.
+Wenn f</t>
+        </r>
+        <r>
+          <rPr>
+            <vertAlign val="subscript"/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>s</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> &gt; 8 ist, gelten Wälzlager als dauerfest.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="93">
   <si>
     <t>INFO</t>
   </si>
@@ -1437,6 +1698,9 @@
   </si>
   <si>
     <t>´--&gt;8,71Mio.km</t>
+  </si>
+  <si>
+    <t>´--&gt;22,6Mio.km</t>
   </si>
 </sst>
 </file>
@@ -2053,6 +2317,117 @@
         <a:xfrm>
           <a:off x="5172075" y="438150"/>
           <a:ext cx="885825" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2952750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5A97DB1-AFBD-4EC0-A296-0F922302BAC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="11011" t="2917" r="14781" b="7162"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="885825" y="1257300"/>
+          <a:ext cx="2828925" cy="1952625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 88" descr="C:\Eigene Dateien\_Peter\Decker16\Icons_Decker16\Lager_02.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5098FCA6-AEE5-42DB-9045-C3086BABCD9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5172075" y="438150"/>
+          <a:ext cx="885825" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2372,8 +2747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF870B6-448D-43DD-89D3-E7ABB130E065}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A71" sqref="A1:D71"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2769,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43845.695129629632</v>
+        <v>43846.520869328706</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2862,7 +3237,7 @@
       <c r="C50" s="21"/>
       <c r="D50" s="35"/>
     </row>
-    <row r="51" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33"/>
       <c r="B51" s="41" t="s">
         <v>60</v>
@@ -3126,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C0479D-85E5-483C-A646-630FF099B2DD}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,7 +3523,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43845.695129629632</v>
+        <v>43846.520869328706</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3648,7 +4023,7 @@
         <v>20865.526124533924</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="43"/>
       <c r="B54" s="41" t="s">
         <v>64</v>
@@ -3839,7 +4214,7 @@
         <v>22952.078736987318</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A70" s="33"/>
       <c r="B70" s="51" t="s">
         <v>87</v>
@@ -3868,4 +4243,752 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39566FE-677C-4469-8A57-F1994027B0D1}">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4">
+        <f ca="1">NOW()</f>
+        <v>43846.520869328706</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="23">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="23">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="24">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="22">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="24">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="28"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="26">
+        <f>(D19+D20)/2</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="33"/>
+      <c r="B38" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="34">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="33"/>
+      <c r="B39" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="35">
+        <f>D38*D28/D23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="33"/>
+      <c r="B40" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="34">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33"/>
+      <c r="B41" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="35">
+        <f>D28/D27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33"/>
+      <c r="B42" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="35" t="e">
+        <f>D30/D29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="33"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="35"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="33"/>
+      <c r="B44" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="39">
+        <f>IF(D27=0,0,IF(D41&gt;D40,0.56,1))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="33"/>
+      <c r="B45" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="34">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33"/>
+      <c r="B46" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="39">
+        <f>IF(D29=0,0,IF(D42&gt;0.8,0.6,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33"/>
+      <c r="B47" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="39">
+        <f>IF(AND(D29=0,D30=0),0,IF(D29=0,1,IF(D42&gt;0.8,0.5,0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="33"/>
+      <c r="B48" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="40">
+        <f>D44*D27+D45*D28</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="33"/>
+      <c r="B49" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="40">
+        <f>D46*D29+D47*D30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="33"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="33"/>
+      <c r="B51" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="21"/>
+      <c r="D51" s="42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="43"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="45">
+        <f>IF(D51="Kugellager",1,IF(D51="Rollenlager",2,0))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="46">
+        <f>IF(D52=1,(D22/D48)^3,IF(D52=2,(D22/D48)^(10/3),0))</f>
+        <v>54163.903883841282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="43"/>
+      <c r="B54" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="47">
+        <f>D53*10^6/(D31*60)</f>
+        <v>452043.9315960714</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="48" t="e">
+        <f>IF(D49&lt;D29,D23/D29,D23/D49)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="33"/>
+      <c r="B56" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="32"/>
+      <c r="D56" s="48" t="e">
+        <f>IF(D55&gt;=1.5,"hoch",IF(AND(D55&gt;=1,D55&lt;1.5),"normal",IF(AND(D55&gt;=0.7,D55&lt;1),"gering","-")))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33"/>
+      <c r="B58" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="33"/>
+      <c r="B59" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="26">
+        <f>D37</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="33"/>
+      <c r="B60" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="49">
+        <f>D31</f>
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33"/>
+      <c r="B61" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="33"/>
+      <c r="B63" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="33"/>
+      <c r="B64" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="40">
+        <f>D63/D61</f>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="33"/>
+      <c r="B65" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="34">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="33"/>
+      <c r="B66" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="35">
+        <f>D65*D24/D48</f>
+        <v>3.6249999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="33"/>
+      <c r="B67" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="22">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="33"/>
+      <c r="B68" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="33"/>
+      <c r="B69" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="50">
+        <f>IF(D68*D67*D53=0,"-",D68*D67*D53)</f>
+        <v>59580.294272225416</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="33"/>
+      <c r="B70" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" s="52">
+        <f>IF(D69="-","-",D69*10^6/(D60*60))</f>
+        <v>497248.32475567865</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="33"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D51" xr:uid="{6A2BEBD9-D361-4A13-A0A9-30E7110D23E6}">
+      <formula1>"Kugellager,Rollenlager"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Lager, neue Werte
</commit_message>
<xml_diff>
--- a/Antriebslager-Berechnungen.xlsx
+++ b/Antriebslager-Berechnungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hopfm.tmb18\Documents\GitHub\KE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F847F3BE-0F4E-46A7-83C8-2C522F900811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E239BF9-2A4E-43C3-ABE2-C9F3EF1BE4C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="2" xr2:uid="{1AF76359-922D-4612-B5D8-8695EF5B153C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{1AF76359-922D-4612-B5D8-8695EF5B153C}"/>
   </bookViews>
   <sheets>
     <sheet name="QJ2" sheetId="1" r:id="rId1"/>
@@ -1965,7 +1965,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -2362,8 +2362,8 @@
     <xf numFmtId="1" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3127,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF870B6-448D-43DD-89D3-E7ABB130E065}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43846.699302546294</v>
+        <v>43850.581097916664</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3283,7 +3283,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="22">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="23">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="23">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="23">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3331,7 +3331,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="23">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3343,7 +3343,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="24">
-        <v>9.4</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="D37" s="26">
         <f>(D19+D20)/2</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D39" s="35">
         <f>D38*D28/D23</f>
-        <v>0.45827737226277376</v>
+        <v>0.48295384615384618</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="D53" s="46">
         <f>IF(D52=1,(D22/D48)^3,IF(D52=2,(D22/D48)^(10/3),0))</f>
-        <v>24774.558525961995</v>
+        <v>21142.596915843027</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3659,11 +3659,11 @@
       </c>
       <c r="D54" s="47">
         <f>D53*10^6/(D31*60)</f>
-        <v>206764.80158539471</v>
+        <v>176452.98711269425</v>
       </c>
       <c r="E54" s="53">
         <f>50*D54</f>
-        <v>10338240.079269735</v>
+        <v>8822649.3556347117</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="D59" s="26">
         <f>D37</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="D66" s="35">
         <f>D65*D24/D48</f>
-        <v>1.4104432821743975</v>
+        <v>1.3654291348709591</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3838,7 +3838,7 @@
       </c>
       <c r="D69" s="50">
         <f>IF(D68*D67*D53=0,"-",D68*D67*D53)</f>
-        <v>27252.014378558197</v>
+        <v>23256.856607427333</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D70" s="52">
         <f>IF(D69="-","-",D69*10^6/(D60*60))</f>
-        <v>227441.2817439342</v>
+        <v>194098.28582396373</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39566FE-677C-4469-8A57-F1994027B0D1}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43846.699302546294</v>
+        <v>43850.581097916664</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4039,7 +4039,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="22">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="23">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4063,7 +4063,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="23">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4075,7 +4075,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="23">
-        <v>221</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4087,7 +4087,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="23">
-        <v>244</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4099,7 +4099,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="24">
-        <v>43.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="D37" s="26">
         <f>(D19+D20)/2</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4373,7 +4373,7 @@
       <c r="C50" s="21"/>
       <c r="D50" s="35"/>
     </row>
-    <row r="51" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33"/>
       <c r="B51" s="41" t="s">
         <v>60</v>
@@ -4402,7 +4402,7 @@
       </c>
       <c r="D53" s="46">
         <f>IF(D52=1,(D22/D48)^3,IF(D52=2,(D22/D48)^(10/3),0))</f>
-        <v>267894.06989424513</v>
+        <v>167620.1726176964</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4415,11 +4415,11 @@
       </c>
       <c r="D54" s="54">
         <f>D53*10^6/(D31*60)</f>
-        <v>2235804.2888853708</v>
+        <v>1398933.1715714941</v>
       </c>
       <c r="E54" s="53">
         <f>50*D54</f>
-        <v>111790214.44426854</v>
+        <v>69946658.578574702</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="D59" s="26">
         <f>D37</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D66" s="35">
         <f>D65*D24/D48</f>
-        <v>5.8557692307692308</v>
+        <v>5.115384615384615</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4594,7 +4594,7 @@
       </c>
       <c r="D69" s="50">
         <f>IF(D68*D67*D53=0,"-",D68*D67*D53)</f>
-        <v>294683.47688366967</v>
+        <v>184382.18987946605</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="D70" s="52">
         <f>IF(D69="-","-",D69*10^6/(D60*60))</f>
-        <v>2459384.7177739083</v>
+        <v>1538826.4887286434</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,8 +4632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC9DC28-B0B8-4E99-9927-5FA4EFEC552D}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43846.699302546294</v>
+        <v>43850.581097916664</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4789,7 +4789,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="22">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4801,7 +4801,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="23">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4813,7 +4813,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="23">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="23">
-        <v>221</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4837,7 +4837,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="23">
-        <v>244</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4849,7 +4849,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="24">
-        <v>43.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="D37" s="26">
         <f>(D19+D20)/2</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="D53" s="46">
         <f>IF(D52=1,(D22/D48)^3,IF(D52=2,(D22/D48)^(10/3),0))</f>
-        <v>545937.9411818739</v>
+        <v>341591.03251363646</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5165,11 +5165,11 @@
       </c>
       <c r="D54" s="54">
         <f>D53*10^6/(D31*60)</f>
-        <v>4556317.3191610239</v>
+        <v>2850868.2399735977</v>
       </c>
       <c r="E54" s="53">
         <f>50*D54</f>
-        <v>227815865.9580512</v>
+        <v>142543411.99867988</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5220,7 +5220,7 @@
       </c>
       <c r="D59" s="26">
         <f>D37</f>
-        <v>110</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5307,7 +5307,7 @@
       </c>
       <c r="D66" s="35">
         <f>D65*D24/D48</f>
-        <v>7.2499999999999991</v>
+        <v>6.3333333333333321</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -5344,7 +5344,7 @@
       </c>
       <c r="D69" s="50">
         <f>IF(D68*D67*D53=0,"-",D68*D67*D53)</f>
-        <v>600531.73530006129</v>
+        <v>375750.13576500013</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5357,7 +5357,7 @@
       </c>
       <c r="D70" s="52">
         <f>IF(D69="-","-",D69*10^6/(D60*60))</f>
-        <v>5011949.0510771265</v>
+        <v>3135955.0639709574</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">NOW()</f>
-        <v>43846.699302546294</v>
+        <v>43850.581097916664</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>